<commit_message>
Affichage pour la création des sondages
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$53</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -210,7 +210,40 @@
     <t>Création des controllers</t>
   </si>
   <si>
-    <t>Renseigner sur les API Resources</t>
+    <t>Congé</t>
+  </si>
+  <si>
+    <t>Ascension</t>
+  </si>
+  <si>
+    <t>Analyse Test</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>Mise en forme du rapport + reécriture de certain points</t>
+  </si>
+  <si>
+    <t>Réfléction sur la stratégie de test et comment la mettre en place</t>
+  </si>
+  <si>
+    <t>Se renseigner sur les API Resources</t>
+  </si>
+  <si>
+    <t>Comprendre le fonctionnement des fichiers resources et les mettre en place</t>
+  </si>
+  <si>
+    <t>Pour le début, ils ne me sont pas trop utile, mais il me servirons plus tard</t>
+  </si>
+  <si>
+    <t>Commencer à mettre en place les fonctionnalitées CRUD + création des affichages pour les sondages</t>
+  </si>
+  <si>
+    <t>Branch Git</t>
+  </si>
+  <si>
+    <t>Création d'une nouvelle branche pour implémenter les fonctionnalitées CRUD</t>
   </si>
 </sst>
 </file>
@@ -854,13 +887,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1197,66 +1230,309 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="10">
+        <v>5</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="10">
         <v>50</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D27" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="10">
-        <v>25</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="B28" s="27"/>
+      <c r="C28" s="10">
+        <v>20</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" s="10"/>
+    </row>
+    <row r="29" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="25">
+        <v>45420</v>
+      </c>
+      <c r="C30" s="5">
+        <v>70</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="5"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="8">
+        <v>60</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" ht="27" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="8">
+        <v>70</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="27" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="8">
+        <v>155</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="10">
+        <v>5</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="10"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="21"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="10"/>
+    </row>
+    <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="10"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="28" t="s">
+      <c r="B38" s="25">
+        <v>45421</v>
+      </c>
+      <c r="C38" s="5">
+        <v>180</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="25">
+        <v>45422</v>
+      </c>
+      <c r="C46" s="5">
+        <v>405</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="10"/>
+    </row>
+    <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="13">
-        <f>MROUND(SUM(C7:C27) /60,0.2)</f>
-        <v>16</v>
-      </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="B53" s="29"/>
+      <c r="C53" s="13">
+        <f>MROUND(SUM(C7:C36) /60,0.2)</f>
+        <v>22</v>
+      </c>
+      <c r="D53" s="14"/>
+      <c r="E53" s="15"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="17">
+    <mergeCell ref="B38:B44"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A53:B53"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="B46:B52"/>
     <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="B21:B28"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:B36"/>
+    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 C14:C19 B21 C21:C27">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C46:C52 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1283,15 +1559,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -1492,17 +1759,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
@@ -1510,14 +1786,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1534,4 +1802,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Création des sondages possible
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$61</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -244,6 +244,18 @@
   </si>
   <si>
     <t>Création d'une nouvelle branche pour implémenter les fonctionnalitées CRUD</t>
+  </si>
+  <si>
+    <t>Affichage Sondage</t>
+  </si>
+  <si>
+    <t>Réaliser la possibilité aux utilisateurs de créer des sondages, ceux-ci gènère directement les questions et les réponses</t>
+  </si>
+  <si>
+    <t>Création de l'affichage des sondages (En cours)</t>
+  </si>
+  <si>
+    <t>Cela m'a pris plus de temps que prévu</t>
   </si>
 </sst>
 </file>
@@ -530,6 +542,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -540,18 +564,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -887,13 +899,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -984,16 +996,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="22">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1008,7 +1020,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1021,7 +1033,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="26"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1034,7 +1046,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="26"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1047,7 +1059,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="26"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1058,7 +1070,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="27"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1067,16 +1079,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="22">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1091,7 +1103,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="26"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1104,7 +1116,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="26"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1117,7 +1129,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1130,7 +1142,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1143,7 +1155,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="27"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1156,16 +1168,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="24"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="25">
+      <c r="B21" s="22">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1180,7 +1192,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="26"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1193,7 +1205,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="26"/>
+      <c r="B23" s="23"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1206,7 +1218,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="26"/>
+      <c r="B24" s="23"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1219,7 +1231,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1232,7 +1244,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="26"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1245,7 +1257,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="26"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1258,7 +1270,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="27"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1271,16 +1283,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="22">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1295,7 +1307,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="26"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1308,7 +1320,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="26"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1323,7 +1335,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="26"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1336,7 +1348,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="26"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1347,14 +1359,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="26"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="27"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1363,16 +1375,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="24"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="25">
+      <c r="B38" s="22">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1385,42 +1397,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="26"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="26"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="26"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="26"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="26"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="27"/>
+      <c r="B44" s="24"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1429,16 +1441,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="22"/>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="24"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="25">
+      <c r="B46" s="22">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1451,72 +1463,161 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="26"/>
+      <c r="B47" s="23"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="26"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="26"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="26"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="26"/>
+      <c r="B51" s="23"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="27"/>
+      <c r="B52" s="24"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="28" t="s">
+    <row r="53" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="25"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="27"/>
+    </row>
+    <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="22">
+        <v>45422</v>
+      </c>
+      <c r="C54" s="5">
+        <v>300</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="8">
+        <v>50</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="8">
+        <v>5</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="23"/>
+      <c r="C57" s="8">
+        <v>5</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="13">
-        <f>MROUND(SUM(C7:C36) /60,0.2)</f>
-        <v>22</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="E53" s="15"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="B61" s="29"/>
+      <c r="C61" s="13">
+        <f>MROUND(SUM(C7:C36,C54:C60) /60,0.2)</f>
+        <v>28</v>
+      </c>
+      <c r="D61" s="14"/>
+      <c r="E61" s="15"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:B60"/>
     <mergeCell ref="B38:B44"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A61:B61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1529,10 +1630,9 @@
     <mergeCell ref="B21:B28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:B36"/>
-    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C46:C52 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 C46:C52 B54 C54:C60">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1559,6 +1659,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -1759,15 +1868,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
   <ds:schemaRefs>
@@ -1786,6 +1886,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1802,12 +1910,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commencer la modification des sondages
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$61</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$69</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>Cela m'a pris plus de temps que prévu</t>
+  </si>
+  <si>
+    <t>Commencer à remplire la partie sur l'implémentation du CRUD</t>
+  </si>
+  <si>
+    <t>Finialiser le création des sondages + permettre la supression des sondages + permettre la modification des éléments</t>
+  </si>
+  <si>
+    <t>Visite du 2ème Expert</t>
   </si>
 </sst>
 </file>
@@ -542,6 +551,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -565,24 +592,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -899,13 +908,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -923,10 +932,10 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="24"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -938,10 +947,10 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="30"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
@@ -953,10 +962,10 @@
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
@@ -968,12 +977,12 @@
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -996,16 +1005,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="28">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1020,7 +1029,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1033,7 +1042,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1046,7 +1055,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="23"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1059,7 +1068,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="23"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1070,7 +1079,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="24"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1079,16 +1088,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="28">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1103,7 +1112,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1116,7 +1125,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="23"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1129,7 +1138,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="23"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1142,7 +1151,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="23"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1155,7 +1164,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="24"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1168,16 +1177,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="28">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1192,7 +1201,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1205,7 +1214,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="23"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1218,7 +1227,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1231,7 +1240,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="23"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1244,7 +1253,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1257,7 +1266,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="23"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1270,7 +1279,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="24"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1283,16 +1292,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="27"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="28">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1307,7 +1316,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="23"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1320,7 +1329,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="23"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1335,7 +1344,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="23"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1348,7 +1357,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="23"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1359,14 +1368,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="23"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="24"/>
+      <c r="B36" s="30"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1375,16 +1384,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="33"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="22">
+      <c r="B38" s="28">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1397,42 +1406,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="23"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="23"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="23"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="23"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="23"/>
+      <c r="B43" s="29"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="24"/>
+      <c r="B44" s="30"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1441,16 +1450,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="27"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="33"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="22">
+      <c r="B46" s="28">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1463,42 +1472,42 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="23"/>
+      <c r="B47" s="29"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="23"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="23"/>
+      <c r="B49" s="29"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="23"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="23"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="24"/>
+      <c r="B52" s="30"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1507,17 +1516,17 @@
       <c r="A53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="27"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="33"/>
     </row>
     <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="22">
-        <v>45422</v>
+      <c r="B54" s="28">
+        <v>45425</v>
       </c>
       <c r="C54" s="5">
         <v>300</v>
@@ -1533,7 +1542,7 @@
       <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="23"/>
+      <c r="B55" s="29"/>
       <c r="C55" s="8">
         <v>50</v>
       </c>
@@ -1546,7 +1555,7 @@
       <c r="A56" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="23"/>
+      <c r="B56" s="29"/>
       <c r="C56" s="8">
         <v>5</v>
       </c>
@@ -1559,7 +1568,7 @@
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="23"/>
+      <c r="B57" s="29"/>
       <c r="C57" s="8">
         <v>5</v>
       </c>
@@ -1570,54 +1579,137 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="23"/>
+      <c r="B58" s="29"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
-      <c r="B59" s="23"/>
+      <c r="B59" s="29"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="24"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="28" t="s">
+    <row r="61" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="31"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="33"/>
+    </row>
+    <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="28">
+        <v>45427</v>
+      </c>
+      <c r="C62" s="5">
+        <v>250</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="5"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="29"/>
+      <c r="C63" s="8">
+        <v>80</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E63" s="8"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B64" s="29"/>
+      <c r="C64" s="8">
+        <v>5</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" s="8"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="29"/>
+      <c r="C65" s="8">
+        <v>25</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="30"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="10"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="13">
-        <f>MROUND(SUM(C7:C36,C54:C60) /60,0.2)</f>
+      <c r="B69" s="23"/>
+      <c r="C69" s="13">
+        <f>MROUND(SUM(C7:C36,C62:C68) /60,0.2)</f>
         <v>28</v>
       </c>
-      <c r="D61" s="14"/>
-      <c r="E61" s="15"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="16" t="s">
+      <c r="D69" s="14"/>
+      <c r="E69" s="15"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:B60"/>
+  <mergeCells count="21">
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:B68"/>
     <mergeCell ref="B38:B44"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A69:B69"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1630,9 +1722,12 @@
     <mergeCell ref="B21:B28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:B36"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:B60"/>
+    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 C46:C52 B54 C54:C60">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B62 C62:C68 C46:C52 B54 C54:C60">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Finir le CRUD pour les sondages
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$69</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$77</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>Visite du 2ème Expert</t>
+  </si>
+  <si>
+    <t>Remplire le journal de travail + Corriger celui de la veille</t>
+  </si>
+  <si>
+    <t>Finir la modification des sondages</t>
+  </si>
+  <si>
+    <t>Documenter la partie de DELETE et UPDATE dans la réalisation</t>
   </si>
 </sst>
 </file>
@@ -551,23 +560,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -581,17 +584,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -908,13 +917,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D66" sqref="D66"/>
+      <selection pane="bottomRight" activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -932,10 +941,10 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="30"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -947,10 +956,10 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
@@ -962,10 +971,10 @@
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
@@ -977,12 +986,12 @@
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1005,16 +1014,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="25">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1029,7 +1038,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1042,7 +1051,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1055,7 +1064,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="29"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1068,7 +1077,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="29"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1079,7 +1088,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="30"/>
+      <c r="B12" s="27"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1088,16 +1097,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="25">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1112,7 +1121,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1125,7 +1134,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="26"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1138,7 +1147,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1151,7 +1160,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1164,7 +1173,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1177,16 +1186,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="24"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="25">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1201,7 +1210,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="29"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1214,7 +1223,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="29"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1227,7 +1236,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="26"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1240,7 +1249,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="29"/>
+      <c r="B25" s="26"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1253,7 +1262,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="26"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1266,7 +1275,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="26"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1279,7 +1288,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1292,16 +1301,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="25">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1316,7 +1325,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="26"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1329,7 +1338,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="26"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1344,7 +1353,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="26"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1357,7 +1366,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="29"/>
+      <c r="B34" s="26"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1368,14 +1377,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="26"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="30"/>
+      <c r="B36" s="27"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1384,16 +1393,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="33"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="25">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1406,42 +1415,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="26"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="29"/>
+      <c r="B40" s="26"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="29"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="29"/>
+      <c r="B42" s="26"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="29"/>
+      <c r="B43" s="26"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="30"/>
+      <c r="B44" s="27"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1450,16 +1459,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="33"/>
+      <c r="B45" s="22"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="24"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="25">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1472,42 +1481,42 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="29"/>
+      <c r="B47" s="26"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="29"/>
+      <c r="B48" s="26"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="29"/>
+      <c r="B49" s="26"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="29"/>
+      <c r="B50" s="26"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="29"/>
+      <c r="B51" s="26"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="30"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1516,16 +1525,16 @@
       <c r="A53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="33"/>
+      <c r="B53" s="22"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="24"/>
     </row>
     <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="25">
         <v>45425</v>
       </c>
       <c r="C54" s="5">
@@ -1542,7 +1551,7 @@
       <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="29"/>
+      <c r="B55" s="26"/>
       <c r="C55" s="8">
         <v>50</v>
       </c>
@@ -1555,7 +1564,7 @@
       <c r="A56" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="26"/>
       <c r="C56" s="8">
         <v>5</v>
       </c>
@@ -1568,7 +1577,7 @@
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="26"/>
       <c r="C57" s="8">
         <v>5</v>
       </c>
@@ -1579,21 +1588,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="29"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
-      <c r="B59" s="29"/>
+      <c r="B59" s="26"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="30"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1602,16 +1611,16 @@
       <c r="A61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="33"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="28">
+      <c r="B62" s="25">
         <v>45427</v>
       </c>
       <c r="C62" s="5">
@@ -1626,7 +1635,7 @@
       <c r="A63" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="29"/>
+      <c r="B63" s="26"/>
       <c r="C63" s="8">
         <v>80</v>
       </c>
@@ -1639,7 +1648,7 @@
       <c r="A64" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="29"/>
+      <c r="B64" s="26"/>
       <c r="C64" s="8">
         <v>5</v>
       </c>
@@ -1652,7 +1661,7 @@
       <c r="A65" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="29"/>
+      <c r="B65" s="26"/>
       <c r="C65" s="8">
         <v>25</v>
       </c>
@@ -1663,53 +1672,126 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
-      <c r="B66" s="29"/>
+      <c r="B66" s="26"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
-      <c r="B67" s="29"/>
+      <c r="B67" s="26"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
-      <c r="B68" s="30"/>
+      <c r="B68" s="27"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="10"/>
     </row>
-    <row r="69" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="22" t="s">
+    <row r="69" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="23"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="24"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" s="25">
+        <v>45428</v>
+      </c>
+      <c r="C70" s="5">
+        <v>85</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" s="26"/>
+      <c r="C71" s="8">
+        <v>90</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B72" s="26"/>
+      <c r="C72" s="8">
+        <v>5</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="10"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="10"/>
+    </row>
+    <row r="76" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="10"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="10"/>
+    </row>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="13">
-        <f>MROUND(SUM(C7:C36,C62:C68) /60,0.2)</f>
-        <v>28</v>
-      </c>
-      <c r="D69" s="14"/>
-      <c r="E69" s="15"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="B77" s="29"/>
+      <c r="C77" s="13">
+        <f>MROUND(SUM(C7:C36,C70:C76) /60,0.2)</f>
+        <v>25</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="E77" s="15"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:B68"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="A69:B69"/>
+  <mergeCells count="23">
+    <mergeCell ref="A77:B77"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1725,9 +1807,16 @@
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="B54:B60"/>
     <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B70:B76"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:B68"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B62 C62:C68 C46:C52 B54 C54:C60">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B70 C70:C76 C46:C52 B54 C54:C60 B62 C62:C68">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -1754,15 +1843,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -1963,6 +2043,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
   <ds:schemaRefs>
@@ -1981,14 +2070,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2005,4 +2086,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Maj de la maquette
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robi\Desktop\survey\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pg78vgj\Desktop\survey\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE25CE23-96BC-47D8-9E75-EB4E952085FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$85</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -294,11 +290,23 @@
   <si>
     <t>https://www.figma.com/design/H1qNDwyQJ5LUQ61ruCoF9L/Survey?t=Za44vT8V6jkkdLHV-1</t>
   </si>
+  <si>
+    <t>Mettre à jour les maquettes dans le rapport</t>
+  </si>
+  <si>
+    <t>Commencer le modifications de l'affichage</t>
+  </si>
+  <si>
+    <t>Correction du MockUp du site + création d'une interface réactive sur figma</t>
+  </si>
+  <si>
+    <t>https://www.figma.com/proto/H1qNDwyQJ5LUQ61ruCoF9L/Survey?t=0IKZ3g8HqjLMEetf-0&amp;scaling=contain&amp;page-id=0%3A1&amp;node-id=12-1922</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -504,7 +512,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -579,23 +587,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -609,19 +615,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -936,17 +948,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
+      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -964,10 +976,10 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="24"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -979,10 +991,10 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
@@ -994,10 +1006,10 @@
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
@@ -1009,12 +1021,12 @@
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1037,16 +1049,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="26">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1061,7 +1073,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="29"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1074,7 +1086,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="29"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1087,7 +1099,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="29"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1100,7 +1112,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="29"/>
+      <c r="B11" s="27"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1111,7 +1123,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="30"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1120,16 +1132,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="26">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1144,7 +1156,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1157,7 +1169,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1170,7 +1182,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1183,7 +1195,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="27"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1196,7 +1208,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1209,16 +1221,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="33"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="26">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1233,7 +1245,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="29"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1246,7 +1258,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="29"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1259,7 +1271,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1272,7 +1284,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="29"/>
+      <c r="B25" s="27"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1285,7 +1297,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="29"/>
+      <c r="B26" s="27"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1298,7 +1310,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="29"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1311,7 +1323,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="30"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1324,16 +1336,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="28">
+      <c r="B30" s="26">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1348,7 +1360,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="29"/>
+      <c r="B31" s="27"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1361,7 +1373,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="27"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1376,7 +1388,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="29"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1389,7 +1401,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="29"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1400,14 +1412,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="30"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1416,16 +1428,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="33"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="25"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="28">
+      <c r="B38" s="26">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1438,42 +1450,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="29"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="29"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="29"/>
+      <c r="B42" s="27"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="29"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="30"/>
+      <c r="B44" s="28"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1482,16 +1494,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="31"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="33"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="25"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="28">
+      <c r="B46" s="26">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1504,42 +1516,42 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="29"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="29"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="29"/>
+      <c r="B49" s="27"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="29"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="29"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="30"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1548,16 +1560,16 @@
       <c r="A53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="33"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="25"/>
     </row>
     <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="28">
+      <c r="B54" s="26">
         <v>45425</v>
       </c>
       <c r="C54" s="5">
@@ -1574,7 +1586,7 @@
       <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="29"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="8">
         <v>50</v>
       </c>
@@ -1587,7 +1599,7 @@
       <c r="A56" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="27"/>
       <c r="C56" s="8">
         <v>5</v>
       </c>
@@ -1600,7 +1612,7 @@
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="8">
         <v>5</v>
       </c>
@@ -1611,21 +1623,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="29"/>
+      <c r="B58" s="27"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
-      <c r="B59" s="29"/>
+      <c r="B59" s="27"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="30"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1634,16 +1646,16 @@
       <c r="A61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="31"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="33"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="24"/>
+      <c r="E61" s="25"/>
     </row>
     <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="28">
+      <c r="B62" s="26">
         <v>45427</v>
       </c>
       <c r="C62" s="5">
@@ -1658,7 +1670,7 @@
       <c r="A63" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="29"/>
+      <c r="B63" s="27"/>
       <c r="C63" s="8">
         <v>80</v>
       </c>
@@ -1671,7 +1683,7 @@
       <c r="A64" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="29"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="8">
         <v>5</v>
       </c>
@@ -1684,7 +1696,7 @@
       <c r="A65" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="29"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="8">
         <v>25</v>
       </c>
@@ -1695,21 +1707,21 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
-      <c r="B66" s="29"/>
+      <c r="B66" s="27"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
-      <c r="B67" s="29"/>
+      <c r="B67" s="27"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
-      <c r="B68" s="30"/>
+      <c r="B68" s="28"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="10"/>
@@ -1718,16 +1730,16 @@
       <c r="A69" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B69" s="31"/>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="33"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="25"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="28">
+      <c r="B70" s="26">
         <v>45428</v>
       </c>
       <c r="C70" s="5">
@@ -1742,7 +1754,7 @@
       <c r="A71" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="29"/>
+      <c r="B71" s="27"/>
       <c r="C71" s="8">
         <v>90</v>
       </c>
@@ -1755,7 +1767,7 @@
       <c r="A72" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="29"/>
+      <c r="B72" s="27"/>
       <c r="C72" s="8">
         <v>5</v>
       </c>
@@ -1766,28 +1778,28 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
-      <c r="B73" s="29"/>
+      <c r="B73" s="27"/>
       <c r="C73" s="8"/>
       <c r="D73" s="11"/>
       <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
-      <c r="B74" s="29"/>
+      <c r="B74" s="27"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="10"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
-      <c r="B75" s="29"/>
+      <c r="B75" s="27"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
-      <c r="B76" s="30"/>
+      <c r="B76" s="28"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="10"/>
@@ -1796,16 +1808,16 @@
       <c r="A77" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B77" s="31"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="33"/>
+      <c r="B77" s="23"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="25"/>
     </row>
     <row r="78" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="28">
+      <c r="B78" s="26">
         <v>45429</v>
       </c>
       <c r="C78" s="5">
@@ -1822,7 +1834,7 @@
       <c r="A79" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="29"/>
+      <c r="B79" s="27"/>
       <c r="C79" s="8">
         <v>110</v>
       </c>
@@ -1835,7 +1847,7 @@
       <c r="A80" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="29"/>
+      <c r="B80" s="27"/>
       <c r="C80" s="8">
         <v>5</v>
       </c>
@@ -1848,70 +1860,147 @@
       <c r="A81" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="29"/>
+      <c r="B81" s="27"/>
       <c r="C81" s="8">
         <v>160</v>
       </c>
       <c r="D81" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E81" s="34" t="s">
+      <c r="E81" s="22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
-      <c r="B82" s="29"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="10"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
-      <c r="B83" s="29"/>
+      <c r="B83" s="27"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
-      <c r="B84" s="30"/>
+      <c r="B84" s="28"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="10"/>
     </row>
-    <row r="85" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="22" t="s">
+    <row r="85" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B85" s="23"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="25"/>
+    </row>
+    <row r="86" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" s="26">
+        <v>45434</v>
+      </c>
+      <c r="C86" s="5">
+        <v>305</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E86" s="35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B87" s="27"/>
+      <c r="C87" s="8">
+        <v>20</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E87" s="8"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" s="27"/>
+      <c r="C88" s="8">
+        <v>30</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E88" s="8"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B89" s="27"/>
+      <c r="C89" s="8">
+        <v>5</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E89" s="22"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="11"/>
+      <c r="E90" s="10"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="10"/>
+    </row>
+    <row r="92" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="10"/>
+      <c r="B92" s="28"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="11"/>
+      <c r="E92" s="10"/>
+    </row>
+    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="13">
-        <f>MROUND(SUM(C7:C36,C78:C84) /60,0.2)</f>
-        <v>28.6</v>
-      </c>
-      <c r="D85" s="14"/>
-      <c r="E85" s="15"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
+      <c r="B93" s="30"/>
+      <c r="C93" s="13">
+        <f>MROUND(SUM(C7:C36,C86:C92) /60,0.2)</f>
+        <v>28</v>
+      </c>
+      <c r="D93" s="14"/>
+      <c r="E93" s="15"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="16"/>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B78:B84"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:B68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:B76"/>
-    <mergeCell ref="A85:B85"/>
+  <mergeCells count="27">
+    <mergeCell ref="A93:B93"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1927,23 +2016,35 @@
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="B54:B60"/>
     <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:B68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B70:B76"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B78:B84"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B78 C78:C84 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B86 C86:C92 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E81" r:id="rId1" xr:uid="{DA1B77BA-CDEA-4C93-B965-A55E192D314F}"/>
+    <hyperlink ref="E81" r:id="rId1"/>
+    <hyperlink ref="E86" r:id="rId2"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="47" orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Etml_font,Normal"&amp;22ETML&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;14&amp;D&amp;R&amp;14Journal</oddFooter>
   </headerFooter>
-  <legacyDrawingHF r:id="rId3"/>
+  <legacyDrawingHF r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1957,6 +2058,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -2157,17 +2269,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
@@ -2177,6 +2278,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2193,21 +2311,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise en place de l'affichage
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>https://www.figma.com/proto/H1qNDwyQJ5LUQ61ruCoF9L/Survey?t=0IKZ3g8HqjLMEetf-0&amp;scaling=contain&amp;page-id=0%3A1&amp;node-id=12-1922</t>
+  </si>
+  <si>
+    <t>Discussion avec le chef de projet sur les points à modifier et les bons points</t>
+  </si>
+  <si>
+    <t>Appliquer les maquettes sur l'application</t>
   </si>
 </sst>
 </file>
@@ -591,6 +597,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -601,40 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -952,13 +958,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E96"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
+      <selection pane="bottomRight" activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -976,10 +982,10 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -991,10 +997,10 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
@@ -1006,10 +1012,10 @@
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
@@ -1021,12 +1027,12 @@
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1049,16 +1055,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="30">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1073,7 +1079,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1086,7 +1092,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="27"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1099,7 +1105,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="27"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1112,7 +1118,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="27"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1123,7 +1129,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="28"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1132,16 +1138,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="25"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="30">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1156,7 +1162,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1169,7 +1175,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1182,7 +1188,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1195,7 +1201,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="27"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1208,7 +1214,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="28"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1221,16 +1227,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="25"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="30">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1245,7 +1251,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="27"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1258,7 +1264,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="27"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1271,7 +1277,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="27"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1284,7 +1290,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="27"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1297,7 +1303,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="27"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1310,7 +1316,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="27"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1323,7 +1329,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="28"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1336,16 +1342,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="25"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="30">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1360,7 +1366,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="27"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1373,7 +1379,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="27"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1388,7 +1394,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="27"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1401,7 +1407,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="27"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1412,14 +1418,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="27"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="28"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1428,16 +1434,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="25"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="26">
+      <c r="B38" s="30">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1450,42 +1456,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="27"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="27"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="27"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="27"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="27"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="28"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1494,16 +1500,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="25"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="35"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B46" s="30">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1516,42 +1522,42 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="27"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="27"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="27"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="27"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="27"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="28"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1560,16 +1566,16 @@
       <c r="A53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="23"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="25"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="35"/>
     </row>
     <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="26">
+      <c r="B54" s="30">
         <v>45425</v>
       </c>
       <c r="C54" s="5">
@@ -1586,7 +1592,7 @@
       <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="27"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="8">
         <v>50</v>
       </c>
@@ -1599,7 +1605,7 @@
       <c r="A56" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="27"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="8">
         <v>5</v>
       </c>
@@ -1612,7 +1618,7 @@
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="27"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="8">
         <v>5</v>
       </c>
@@ -1623,21 +1629,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="27"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
-      <c r="B59" s="27"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="28"/>
+      <c r="B60" s="32"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1646,16 +1652,16 @@
       <c r="A61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="23"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="25"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="35"/>
     </row>
     <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="26">
+      <c r="B62" s="30">
         <v>45427</v>
       </c>
       <c r="C62" s="5">
@@ -1670,7 +1676,7 @@
       <c r="A63" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="27"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="8">
         <v>80</v>
       </c>
@@ -1683,7 +1689,7 @@
       <c r="A64" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="27"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="8">
         <v>5</v>
       </c>
@@ -1696,7 +1702,7 @@
       <c r="A65" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="27"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="8">
         <v>25</v>
       </c>
@@ -1707,21 +1713,21 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
-      <c r="B66" s="27"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
-      <c r="B67" s="27"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
-      <c r="B68" s="28"/>
+      <c r="B68" s="32"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="10"/>
@@ -1730,16 +1736,16 @@
       <c r="A69" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B69" s="23"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="25"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="35"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="26">
+      <c r="B70" s="30">
         <v>45428</v>
       </c>
       <c r="C70" s="5">
@@ -1754,7 +1760,7 @@
       <c r="A71" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="27"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="8">
         <v>90</v>
       </c>
@@ -1767,7 +1773,7 @@
       <c r="A72" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="27"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="8">
         <v>5</v>
       </c>
@@ -1778,28 +1784,28 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
-      <c r="B73" s="27"/>
+      <c r="B73" s="31"/>
       <c r="C73" s="8"/>
       <c r="D73" s="11"/>
       <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
-      <c r="B74" s="27"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="10"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
-      <c r="B75" s="27"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
-      <c r="B76" s="28"/>
+      <c r="B76" s="32"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="10"/>
@@ -1808,16 +1814,16 @@
       <c r="A77" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B77" s="23"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="25"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="35"/>
     </row>
     <row r="78" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="26">
+      <c r="B78" s="30">
         <v>45429</v>
       </c>
       <c r="C78" s="5">
@@ -1834,7 +1840,7 @@
       <c r="A79" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="27"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="8">
         <v>110</v>
       </c>
@@ -1847,7 +1853,7 @@
       <c r="A80" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="27"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="8">
         <v>5</v>
       </c>
@@ -1860,7 +1866,7 @@
       <c r="A81" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="27"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="8">
         <v>160</v>
       </c>
@@ -1873,21 +1879,21 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
-      <c r="B82" s="27"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="10"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
-      <c r="B83" s="27"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
-      <c r="B84" s="28"/>
+      <c r="B84" s="32"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="10"/>
@@ -1896,16 +1902,16 @@
       <c r="A85" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="25"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="35"/>
     </row>
     <row r="86" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="26">
+      <c r="B86" s="30">
         <v>45434</v>
       </c>
       <c r="C86" s="5">
@@ -1914,7 +1920,7 @@
       <c r="D86" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E86" s="35" t="s">
+      <c r="E86" s="23" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1922,7 +1928,7 @@
       <c r="A87" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B87" s="27"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="8">
         <v>20</v>
       </c>
@@ -1935,7 +1941,7 @@
       <c r="A88" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B88" s="27"/>
+      <c r="B88" s="31"/>
       <c r="C88" s="8">
         <v>30</v>
       </c>
@@ -1948,7 +1954,7 @@
       <c r="A89" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B89" s="27"/>
+      <c r="B89" s="31"/>
       <c r="C89" s="8">
         <v>5</v>
       </c>
@@ -1959,48 +1965,139 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
-      <c r="B90" s="27"/>
+      <c r="B90" s="31"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
       <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
-      <c r="B91" s="27"/>
+      <c r="B91" s="31"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="10"/>
     </row>
     <row r="92" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
-      <c r="B92" s="28"/>
+      <c r="B92" s="32"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
       <c r="E92" s="10"/>
     </row>
-    <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="29" t="s">
+    <row r="93" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B93" s="33"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="35"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B94" s="30">
+        <v>45435</v>
+      </c>
+      <c r="C94" s="5">
+        <v>20</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E94" s="23"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" s="31"/>
+      <c r="C95" s="8">
+        <v>155</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E95" s="8"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" s="31"/>
+      <c r="C96" s="8">
+        <v>5</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E96" s="8"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="21"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="11"/>
+      <c r="E97" s="22"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="21"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="11"/>
+      <c r="E98" s="10"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="21"/>
+      <c r="B99" s="31"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="11"/>
+      <c r="E99" s="10"/>
+    </row>
+    <row r="100" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="10"/>
+      <c r="B100" s="32"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="11"/>
+      <c r="E100" s="10"/>
+    </row>
+    <row r="101" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B93" s="30"/>
-      <c r="C93" s="13">
-        <f>MROUND(SUM(C7:C36,C86:C92) /60,0.2)</f>
-        <v>28</v>
-      </c>
-      <c r="D93" s="14"/>
-      <c r="E93" s="15"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="16" t="s">
+      <c r="B101" s="25"/>
+      <c r="C101" s="13">
+        <f>MROUND(SUM(C7:C36,C94:C100) /60,0.2)</f>
+        <v>25</v>
+      </c>
+      <c r="D101" s="14"/>
+      <c r="E101" s="15"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A93:B93"/>
+  <mergeCells count="29">
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="B94:B100"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:B68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B70:B76"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B78:B84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="A101:B101"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -2016,20 +2113,9 @@
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="B54:B60"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:B68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:B76"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B78:B84"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B86 C86:C92 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B94 C94:C100 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84 B86 C86:C92">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2058,17 +2144,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -2269,6 +2344,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
@@ -2278,23 +2364,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2311,4 +2380,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Création des roles admin et user
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="97">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -325,6 +325,18 @@
   </si>
   <si>
     <t>ca</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Mettre à jour les tests existants</t>
+  </si>
+  <si>
+    <t>Gestion rôles</t>
+  </si>
+  <si>
+    <t>Commencer la gestion des roles + création de l'interface Admin (En cours)</t>
   </si>
 </sst>
 </file>
@@ -619,6 +631,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -630,36 +672,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -984,13 +996,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E111"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D85" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D99" sqref="D99"/>
+      <selection pane="bottomRight" activeCell="D112" sqref="D112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1008,10 +1020,10 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1023,10 +1035,10 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
@@ -1038,10 +1050,10 @@
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
@@ -1053,12 +1065,12 @@
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1081,16 +1093,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="30">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1105,7 +1117,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="31"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1118,7 +1130,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="28"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1131,7 +1143,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="28"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1144,7 +1156,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="28"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1155,7 +1167,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="29"/>
+      <c r="B12" s="32"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1164,16 +1176,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="30">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1188,7 +1200,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1201,7 +1213,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1214,7 +1226,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1227,7 +1239,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="28"/>
+      <c r="B18" s="31"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1240,7 +1252,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1253,16 +1265,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="35"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="30">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1277,7 +1289,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="28"/>
+      <c r="B22" s="31"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1290,7 +1302,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="28"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1303,7 +1315,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="28"/>
+      <c r="B24" s="31"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1316,7 +1328,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1329,7 +1341,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="31"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1342,7 +1354,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="28"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1355,7 +1367,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="29"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1368,16 +1380,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="35"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="30">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1392,7 +1404,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="28"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1405,7 +1417,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="28"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1420,7 +1432,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="28"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1433,7 +1445,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="28"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1444,14 +1456,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="28"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1460,16 +1472,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="35"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="27">
+      <c r="B38" s="30">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1482,42 +1494,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="31"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="28"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="28"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="28"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="29"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1526,16 +1538,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="26"/>
+      <c r="B45" s="33"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="35"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="27">
+      <c r="B46" s="30">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1548,42 +1560,42 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="28"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="28"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="28"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="28"/>
+      <c r="B50" s="31"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="28"/>
+      <c r="B51" s="31"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="29"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1592,16 +1604,16 @@
       <c r="A53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="26"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="35"/>
     </row>
     <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="27">
+      <c r="B54" s="30">
         <v>45425</v>
       </c>
       <c r="C54" s="5">
@@ -1618,7 +1630,7 @@
       <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="28"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="8">
         <v>50</v>
       </c>
@@ -1631,7 +1643,7 @@
       <c r="A56" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="28"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="8">
         <v>5</v>
       </c>
@@ -1644,7 +1656,7 @@
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="28"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="8">
         <v>5</v>
       </c>
@@ -1655,21 +1667,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="28"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
-      <c r="B59" s="28"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="29"/>
+      <c r="B60" s="32"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1678,16 +1690,16 @@
       <c r="A61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="24"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="26"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="35"/>
     </row>
     <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="27">
+      <c r="B62" s="30">
         <v>45427</v>
       </c>
       <c r="C62" s="5">
@@ -1702,7 +1714,7 @@
       <c r="A63" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="28"/>
+      <c r="B63" s="31"/>
       <c r="C63" s="8">
         <v>80</v>
       </c>
@@ -1715,7 +1727,7 @@
       <c r="A64" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="28"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="8">
         <v>5</v>
       </c>
@@ -1728,7 +1740,7 @@
       <c r="A65" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="28"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="8">
         <v>25</v>
       </c>
@@ -1739,21 +1751,21 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
-      <c r="B66" s="28"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
-      <c r="B67" s="28"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
-      <c r="B68" s="29"/>
+      <c r="B68" s="32"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="10"/>
@@ -1762,16 +1774,16 @@
       <c r="A69" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="25"/>
-      <c r="D69" s="25"/>
-      <c r="E69" s="26"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="35"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="27">
+      <c r="B70" s="30">
         <v>45428</v>
       </c>
       <c r="C70" s="5">
@@ -1786,7 +1798,7 @@
       <c r="A71" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="28"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="8">
         <v>90</v>
       </c>
@@ -1799,7 +1811,7 @@
       <c r="A72" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="28"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="8">
         <v>5</v>
       </c>
@@ -1810,28 +1822,28 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
-      <c r="B73" s="28"/>
+      <c r="B73" s="31"/>
       <c r="C73" s="8"/>
       <c r="D73" s="11"/>
       <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
-      <c r="B74" s="28"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="10"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
-      <c r="B75" s="28"/>
+      <c r="B75" s="31"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
-      <c r="B76" s="29"/>
+      <c r="B76" s="32"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="10"/>
@@ -1840,16 +1852,16 @@
       <c r="A77" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="25"/>
-      <c r="E77" s="26"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="35"/>
     </row>
     <row r="78" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="27">
+      <c r="B78" s="30">
         <v>45429</v>
       </c>
       <c r="C78" s="5">
@@ -1866,7 +1878,7 @@
       <c r="A79" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="28"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="8">
         <v>110</v>
       </c>
@@ -1879,7 +1891,7 @@
       <c r="A80" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="28"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="8">
         <v>5</v>
       </c>
@@ -1892,7 +1904,7 @@
       <c r="A81" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="28"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="8">
         <v>160</v>
       </c>
@@ -1905,21 +1917,21 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
-      <c r="B82" s="28"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="10"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
-      <c r="B83" s="28"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
-      <c r="B84" s="29"/>
+      <c r="B84" s="32"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="10"/>
@@ -1928,16 +1940,16 @@
       <c r="A85" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="26"/>
+      <c r="B85" s="33"/>
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="35"/>
     </row>
     <row r="86" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B86" s="30">
         <v>45434</v>
       </c>
       <c r="C86" s="5">
@@ -1954,7 +1966,7 @@
       <c r="A87" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B87" s="28"/>
+      <c r="B87" s="31"/>
       <c r="C87" s="8">
         <v>20</v>
       </c>
@@ -1967,7 +1979,7 @@
       <c r="A88" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B88" s="28"/>
+      <c r="B88" s="31"/>
       <c r="C88" s="8">
         <v>30</v>
       </c>
@@ -1980,7 +1992,7 @@
       <c r="A89" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B89" s="28"/>
+      <c r="B89" s="31"/>
       <c r="C89" s="8">
         <v>5</v>
       </c>
@@ -1991,21 +2003,21 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
-      <c r="B90" s="28"/>
+      <c r="B90" s="31"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
       <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
-      <c r="B91" s="28"/>
+      <c r="B91" s="31"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="10"/>
     </row>
     <row r="92" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
-      <c r="B92" s="29"/>
+      <c r="B92" s="32"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
       <c r="E92" s="10"/>
@@ -2014,16 +2026,16 @@
       <c r="A93" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="25"/>
-      <c r="D93" s="25"/>
-      <c r="E93" s="26"/>
+      <c r="B93" s="33"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="35"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B94" s="27">
+      <c r="B94" s="30">
         <v>45435</v>
       </c>
       <c r="C94" s="5">
@@ -2092,16 +2104,16 @@
       <c r="A101" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B101" s="24"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="26"/>
+      <c r="B101" s="33"/>
+      <c r="C101" s="34"/>
+      <c r="D101" s="34"/>
+      <c r="E101" s="35"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B102" s="27">
+      <c r="B102" s="30">
         <v>45436</v>
       </c>
       <c r="C102" s="5">
@@ -2118,7 +2130,7 @@
       <c r="A103" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B103" s="28"/>
+      <c r="B103" s="31"/>
       <c r="C103" s="8">
         <v>190</v>
       </c>
@@ -2133,7 +2145,7 @@
       <c r="A104" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B104" s="28"/>
+      <c r="B104" s="31"/>
       <c r="C104" s="8">
         <v>160</v>
       </c>
@@ -2146,7 +2158,7 @@
       <c r="A105" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B105" s="28"/>
+      <c r="B105" s="31"/>
       <c r="C105" s="8">
         <v>5</v>
       </c>
@@ -2157,48 +2169,143 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
-      <c r="B106" s="28"/>
+      <c r="B106" s="31"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
       <c r="E106" s="10"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
-      <c r="B107" s="28"/>
+      <c r="B107" s="31"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
       <c r="E107" s="10"/>
     </row>
     <row r="108" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10"/>
-      <c r="B108" s="29"/>
+      <c r="B108" s="32"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
       <c r="E108" s="10"/>
     </row>
-    <row r="109" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="30" t="s">
+    <row r="109" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B109" s="33"/>
+      <c r="C109" s="34"/>
+      <c r="D109" s="34"/>
+      <c r="E109" s="35"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B110" s="30">
+        <v>45439</v>
+      </c>
+      <c r="C110" s="5">
+        <v>30</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E110" s="10"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B111" s="31"/>
+      <c r="C111" s="8">
+        <v>190</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E111" s="22"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B112" s="31"/>
+      <c r="C112" s="8">
+        <v>5</v>
+      </c>
+      <c r="D112" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E112" s="8"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="21"/>
+      <c r="B113" s="31"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="22"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="21"/>
+      <c r="B114" s="31"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="10"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="21"/>
+      <c r="B115" s="31"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="10"/>
+    </row>
+    <row r="116" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="10"/>
+      <c r="B116" s="32"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="10"/>
+    </row>
+    <row r="117" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B109" s="31"/>
-      <c r="C109" s="13">
-        <f>MROUND(SUM(C7:C36,C54:C108) /60,0.2)</f>
-        <v>59.400000000000006</v>
-      </c>
-      <c r="D109" s="14"/>
-      <c r="E109" s="15"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="16" t="s">
+      <c r="B117" s="25"/>
+      <c r="C117" s="13">
+        <f>MROUND(SUM(C7:C36,C54:C116) /60,0.2)</f>
+        <v>63.2</v>
+      </c>
+      <c r="D117" s="14"/>
+      <c r="E117" s="15"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="16"/>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A109:B109"/>
+  <mergeCells count="33">
+    <mergeCell ref="B102:B108"/>
+    <mergeCell ref="B109:E109"/>
+    <mergeCell ref="B110:B116"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B61:E61"/>
+    <mergeCell ref="B62:B68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B70:B76"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B78:B84"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="B94:B100"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="A117:B117"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -2214,24 +2321,9 @@
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="B54:B60"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="B102:B108"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B14:B19"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B62:B68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B70:B76"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B78:B84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="B94:B100"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B102 C102:C108 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84 B86 C86:C92 B94 C94:C100">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B110 C110:C116 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84 B86 C86:C92 B94 C94:C100 B102 C102:C108">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2242,7 +2334,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="42" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Etml_font,Normal"&amp;22ETML&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;14&amp;D&amp;R&amp;14Journal</oddFooter>
@@ -2261,17 +2353,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -2472,6 +2553,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
@@ -2481,23 +2573,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2514,4 +2589,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Commencer l'affichage des réponse
</commit_message>
<xml_diff>
--- a/doc/JdT.xlsx
+++ b/doc/JdT.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="109">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -355,6 +355,24 @@
   </si>
   <si>
     <t>Commencer l'exportation PDF</t>
+  </si>
+  <si>
+    <t>Export Excel</t>
+  </si>
+  <si>
+    <t>Affichage réponse</t>
+  </si>
+  <si>
+    <t>Commenter la partie Export PDF et la partie Export Excel</t>
+  </si>
+  <si>
+    <t>Finaliser l'exportation PDF</t>
+  </si>
+  <si>
+    <t>Permettre à l'utilisateur d'exporter les utilisateurs sous format Excel</t>
+  </si>
+  <si>
+    <t>Commencer l'affichage des réponse du formulaires</t>
   </si>
 </sst>
 </file>
@@ -649,6 +667,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -661,17 +691,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,24 +716,6 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1014,13 +1032,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E135"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D123" sqref="D123"/>
+      <selection pane="bottomRight" activeCell="E126" sqref="E126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1038,10 +1056,10 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="20" t="s">
         <v>1</v>
       </c>
@@ -1053,10 +1071,10 @@
       <c r="A2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
@@ -1068,10 +1086,10 @@
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="20" t="s">
         <v>16</v>
       </c>
@@ -1083,12 +1101,12 @@
       <c r="A4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1111,16 +1129,16 @@
       <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="27">
         <v>45414</v>
       </c>
       <c r="C7" s="5">
@@ -1135,7 +1153,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="25"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="8">
         <v>30</v>
       </c>
@@ -1148,7 +1166,7 @@
       <c r="A9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="25"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8">
         <v>15</v>
       </c>
@@ -1161,7 +1179,7 @@
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="25"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="8">
         <v>10</v>
       </c>
@@ -1174,7 +1192,7 @@
       <c r="A11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="25"/>
+      <c r="B11" s="28"/>
       <c r="C11" s="10">
         <v>75</v>
       </c>
@@ -1185,7 +1203,7 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
-      <c r="B12" s="26"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
       <c r="E12" s="10"/>
@@ -1194,16 +1212,16 @@
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="29"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="27">
         <v>45415</v>
       </c>
       <c r="C14" s="5">
@@ -1218,7 +1236,7 @@
       <c r="A15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="25"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8">
         <v>150</v>
       </c>
@@ -1231,7 +1249,7 @@
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="25"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="8">
         <v>90</v>
       </c>
@@ -1244,7 +1262,7 @@
       <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="8">
         <v>25</v>
       </c>
@@ -1257,7 +1275,7 @@
       <c r="A18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="25"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="10">
         <v>120</v>
       </c>
@@ -1270,7 +1288,7 @@
       <c r="A19" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="26"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="10">
         <v>5</v>
       </c>
@@ -1283,16 +1301,16 @@
       <c r="A20" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="27">
         <v>45418</v>
       </c>
       <c r="C21" s="5">
@@ -1307,7 +1325,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="25"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="8">
         <v>45</v>
       </c>
@@ -1320,7 +1338,7 @@
       <c r="A23" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="25"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="8">
         <v>160</v>
       </c>
@@ -1333,7 +1351,7 @@
       <c r="A24" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="25"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="8">
         <v>5</v>
       </c>
@@ -1346,7 +1364,7 @@
       <c r="A25" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="10">
         <v>5</v>
       </c>
@@ -1359,7 +1377,7 @@
       <c r="A26" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="25"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="10">
         <v>5</v>
       </c>
@@ -1372,7 +1390,7 @@
       <c r="A27" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="25"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="10">
         <v>50</v>
       </c>
@@ -1385,7 +1403,7 @@
       <c r="A28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="26"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="10">
         <v>20</v>
       </c>
@@ -1398,16 +1416,16 @@
       <c r="A29" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="24">
+      <c r="B30" s="27">
         <v>45420</v>
       </c>
       <c r="C30" s="5">
@@ -1422,7 +1440,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="25"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="8">
         <v>60</v>
       </c>
@@ -1435,7 +1453,7 @@
       <c r="A32" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="25"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="8">
         <v>70</v>
       </c>
@@ -1450,7 +1468,7 @@
       <c r="A33" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="25"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="8">
         <v>155</v>
       </c>
@@ -1463,7 +1481,7 @@
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="25"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="10">
         <v>5</v>
       </c>
@@ -1474,14 +1492,14 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
-      <c r="B35" s="25"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="10"/>
       <c r="D35" s="11"/>
       <c r="E35" s="10"/>
     </row>
     <row r="36" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
-      <c r="B36" s="26"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="10"/>
@@ -1490,16 +1508,16 @@
       <c r="A37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="29"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="24">
+      <c r="B38" s="27">
         <v>45421</v>
       </c>
       <c r="C38" s="5">
@@ -1512,42 +1530,42 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="25"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="25"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="25"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
-      <c r="B42" s="25"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
-      <c r="B43" s="25"/>
+      <c r="B43" s="28"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="10"/>
     </row>
     <row r="44" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
-      <c r="B44" s="26"/>
+      <c r="B44" s="29"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
       <c r="E44" s="10"/>
@@ -1556,16 +1574,16 @@
       <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="29"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="26"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="24">
+      <c r="B46" s="27">
         <v>45422</v>
       </c>
       <c r="C46" s="5">
@@ -1578,42 +1596,42 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="25"/>
+      <c r="B47" s="28"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
-      <c r="B48" s="25"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="8"/>
       <c r="D48" s="9"/>
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
-      <c r="B49" s="25"/>
+      <c r="B49" s="28"/>
       <c r="C49" s="8"/>
       <c r="D49" s="9"/>
       <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="21"/>
-      <c r="B50" s="25"/>
+      <c r="B50" s="28"/>
       <c r="C50" s="10"/>
       <c r="D50" s="11"/>
       <c r="E50" s="10"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
-      <c r="B51" s="25"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="10"/>
       <c r="D51" s="11"/>
       <c r="E51" s="10"/>
     </row>
     <row r="52" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
-      <c r="B52" s="26"/>
+      <c r="B52" s="29"/>
       <c r="C52" s="10"/>
       <c r="D52" s="11"/>
       <c r="E52" s="10"/>
@@ -1622,16 +1640,16 @@
       <c r="A53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="26"/>
     </row>
     <row r="54" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="24">
+      <c r="B54" s="27">
         <v>45425</v>
       </c>
       <c r="C54" s="5">
@@ -1648,7 +1666,7 @@
       <c r="A55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="28"/>
       <c r="C55" s="8">
         <v>50</v>
       </c>
@@ -1661,7 +1679,7 @@
       <c r="A56" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="25"/>
+      <c r="B56" s="28"/>
       <c r="C56" s="8">
         <v>5</v>
       </c>
@@ -1674,7 +1692,7 @@
       <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B57" s="25"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="8">
         <v>5</v>
       </c>
@@ -1685,21 +1703,21 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
-      <c r="B58" s="25"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="10"/>
       <c r="D58" s="11"/>
       <c r="E58" s="10"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
-      <c r="B59" s="25"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="10"/>
       <c r="D59" s="11"/>
       <c r="E59" s="10"/>
     </row>
     <row r="60" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="26"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1708,16 +1726,16 @@
       <c r="A61" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="29"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="25"/>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="24">
+      <c r="B62" s="27">
         <v>45427</v>
       </c>
       <c r="C62" s="5">
@@ -1732,7 +1750,7 @@
       <c r="A63" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B63" s="25"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="8">
         <v>80</v>
       </c>
@@ -1745,7 +1763,7 @@
       <c r="A64" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B64" s="25"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="8">
         <v>5</v>
       </c>
@@ -1758,7 +1776,7 @@
       <c r="A65" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B65" s="25"/>
+      <c r="B65" s="28"/>
       <c r="C65" s="8">
         <v>25</v>
       </c>
@@ -1769,21 +1787,21 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
-      <c r="B66" s="25"/>
+      <c r="B66" s="28"/>
       <c r="C66" s="10"/>
       <c r="D66" s="11"/>
       <c r="E66" s="10"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
-      <c r="B67" s="25"/>
+      <c r="B67" s="28"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="10"/>
     </row>
     <row r="68" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="10"/>
-      <c r="B68" s="26"/>
+      <c r="B68" s="29"/>
       <c r="C68" s="10"/>
       <c r="D68" s="11"/>
       <c r="E68" s="10"/>
@@ -1792,16 +1810,16 @@
       <c r="A69" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B69" s="27"/>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="29"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="25"/>
+      <c r="D69" s="25"/>
+      <c r="E69" s="26"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="24">
+      <c r="B70" s="27">
         <v>45428</v>
       </c>
       <c r="C70" s="5">
@@ -1816,7 +1834,7 @@
       <c r="A71" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="25"/>
+      <c r="B71" s="28"/>
       <c r="C71" s="8">
         <v>90</v>
       </c>
@@ -1829,7 +1847,7 @@
       <c r="A72" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="25"/>
+      <c r="B72" s="28"/>
       <c r="C72" s="8">
         <v>5</v>
       </c>
@@ -1840,28 +1858,28 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="21"/>
-      <c r="B73" s="25"/>
+      <c r="B73" s="28"/>
       <c r="C73" s="8"/>
       <c r="D73" s="11"/>
       <c r="E73" s="8"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
-      <c r="B74" s="25"/>
+      <c r="B74" s="28"/>
       <c r="C74" s="10"/>
       <c r="D74" s="11"/>
       <c r="E74" s="10"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
-      <c r="B75" s="25"/>
+      <c r="B75" s="28"/>
       <c r="C75" s="10"/>
       <c r="D75" s="11"/>
       <c r="E75" s="10"/>
     </row>
     <row r="76" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="10"/>
-      <c r="B76" s="26"/>
+      <c r="B76" s="29"/>
       <c r="C76" s="10"/>
       <c r="D76" s="11"/>
       <c r="E76" s="10"/>
@@ -1870,16 +1888,16 @@
       <c r="A77" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B77" s="27"/>
-      <c r="C77" s="28"/>
-      <c r="D77" s="28"/>
-      <c r="E77" s="29"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="26"/>
     </row>
     <row r="78" spans="1:5" ht="27" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="24">
+      <c r="B78" s="27">
         <v>45429</v>
       </c>
       <c r="C78" s="5">
@@ -1896,7 +1914,7 @@
       <c r="A79" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B79" s="25"/>
+      <c r="B79" s="28"/>
       <c r="C79" s="8">
         <v>110</v>
       </c>
@@ -1909,7 +1927,7 @@
       <c r="A80" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="25"/>
+      <c r="B80" s="28"/>
       <c r="C80" s="8">
         <v>5</v>
       </c>
@@ -1922,7 +1940,7 @@
       <c r="A81" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B81" s="25"/>
+      <c r="B81" s="28"/>
       <c r="C81" s="8">
         <v>160</v>
       </c>
@@ -1935,21 +1953,21 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="21"/>
-      <c r="B82" s="25"/>
+      <c r="B82" s="28"/>
       <c r="C82" s="10"/>
       <c r="D82" s="11"/>
       <c r="E82" s="10"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
-      <c r="B83" s="25"/>
+      <c r="B83" s="28"/>
       <c r="C83" s="10"/>
       <c r="D83" s="11"/>
       <c r="E83" s="10"/>
     </row>
     <row r="84" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="10"/>
-      <c r="B84" s="26"/>
+      <c r="B84" s="29"/>
       <c r="C84" s="10"/>
       <c r="D84" s="11"/>
       <c r="E84" s="10"/>
@@ -1958,16 +1976,16 @@
       <c r="A85" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B85" s="27"/>
-      <c r="C85" s="28"/>
-      <c r="D85" s="28"/>
-      <c r="E85" s="29"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="25"/>
+      <c r="D85" s="25"/>
+      <c r="E85" s="26"/>
     </row>
     <row r="86" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="24">
+      <c r="B86" s="27">
         <v>45434</v>
       </c>
       <c r="C86" s="5">
@@ -1984,7 +2002,7 @@
       <c r="A87" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B87" s="25"/>
+      <c r="B87" s="28"/>
       <c r="C87" s="8">
         <v>20</v>
       </c>
@@ -1997,7 +2015,7 @@
       <c r="A88" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B88" s="25"/>
+      <c r="B88" s="28"/>
       <c r="C88" s="8">
         <v>30</v>
       </c>
@@ -2010,7 +2028,7 @@
       <c r="A89" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B89" s="25"/>
+      <c r="B89" s="28"/>
       <c r="C89" s="8">
         <v>5</v>
       </c>
@@ -2021,21 +2039,21 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="21"/>
-      <c r="B90" s="25"/>
+      <c r="B90" s="28"/>
       <c r="C90" s="10"/>
       <c r="D90" s="11"/>
       <c r="E90" s="10"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="21"/>
-      <c r="B91" s="25"/>
+      <c r="B91" s="28"/>
       <c r="C91" s="10"/>
       <c r="D91" s="11"/>
       <c r="E91" s="10"/>
     </row>
     <row r="92" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="10"/>
-      <c r="B92" s="26"/>
+      <c r="B92" s="29"/>
       <c r="C92" s="10"/>
       <c r="D92" s="11"/>
       <c r="E92" s="10"/>
@@ -2044,16 +2062,16 @@
       <c r="A93" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B93" s="27"/>
-      <c r="C93" s="28"/>
-      <c r="D93" s="28"/>
-      <c r="E93" s="29"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="25"/>
+      <c r="D93" s="25"/>
+      <c r="E93" s="26"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B94" s="24">
+      <c r="B94" s="27">
         <v>45435</v>
       </c>
       <c r="C94" s="5">
@@ -2068,7 +2086,7 @@
       <c r="A95" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B95" s="30"/>
+      <c r="B95" s="36"/>
       <c r="C95" s="8">
         <v>155</v>
       </c>
@@ -2081,7 +2099,7 @@
       <c r="A96" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B96" s="30"/>
+      <c r="B96" s="36"/>
       <c r="C96" s="8">
         <v>5</v>
       </c>
@@ -2092,28 +2110,28 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="21"/>
-      <c r="B97" s="30"/>
+      <c r="B97" s="36"/>
       <c r="C97" s="8"/>
       <c r="D97" s="11"/>
       <c r="E97" s="22"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="21"/>
-      <c r="B98" s="30"/>
+      <c r="B98" s="36"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
       <c r="E98" s="10"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="21"/>
-      <c r="B99" s="30"/>
+      <c r="B99" s="36"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
       <c r="E99" s="10"/>
     </row>
     <row r="100" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="10"/>
-      <c r="B100" s="31"/>
+      <c r="B100" s="37"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
       <c r="E100" s="10"/>
@@ -2122,16 +2140,16 @@
       <c r="A101" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B101" s="27"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="29"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="26"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B102" s="24">
+      <c r="B102" s="27">
         <v>45436</v>
       </c>
       <c r="C102" s="5">
@@ -2148,7 +2166,7 @@
       <c r="A103" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B103" s="25"/>
+      <c r="B103" s="28"/>
       <c r="C103" s="8">
         <v>190</v>
       </c>
@@ -2163,7 +2181,7 @@
       <c r="A104" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B104" s="25"/>
+      <c r="B104" s="28"/>
       <c r="C104" s="8">
         <v>160</v>
       </c>
@@ -2176,7 +2194,7 @@
       <c r="A105" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B105" s="25"/>
+      <c r="B105" s="28"/>
       <c r="C105" s="8">
         <v>5</v>
       </c>
@@ -2187,21 +2205,21 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="21"/>
-      <c r="B106" s="25"/>
+      <c r="B106" s="28"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
       <c r="E106" s="10"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="21"/>
-      <c r="B107" s="25"/>
+      <c r="B107" s="28"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
       <c r="E107" s="10"/>
     </row>
     <row r="108" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="10"/>
-      <c r="B108" s="26"/>
+      <c r="B108" s="29"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
       <c r="E108" s="10"/>
@@ -2210,16 +2228,16 @@
       <c r="A109" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B109" s="27"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="29"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="25"/>
+      <c r="D109" s="25"/>
+      <c r="E109" s="26"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B110" s="24">
+      <c r="B110" s="27">
         <v>45439</v>
       </c>
       <c r="C110" s="5">
@@ -2234,7 +2252,7 @@
       <c r="A111" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B111" s="25"/>
+      <c r="B111" s="28"/>
       <c r="C111" s="8">
         <v>190</v>
       </c>
@@ -2247,7 +2265,7 @@
       <c r="A112" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B112" s="25"/>
+      <c r="B112" s="28"/>
       <c r="C112" s="8">
         <v>5</v>
       </c>
@@ -2258,28 +2276,28 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="21"/>
-      <c r="B113" s="25"/>
+      <c r="B113" s="28"/>
       <c r="C113" s="8"/>
       <c r="D113" s="11"/>
       <c r="E113" s="22"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="21"/>
-      <c r="B114" s="25"/>
+      <c r="B114" s="28"/>
       <c r="C114" s="10"/>
       <c r="D114" s="11"/>
       <c r="E114" s="10"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="21"/>
-      <c r="B115" s="25"/>
+      <c r="B115" s="28"/>
       <c r="C115" s="10"/>
       <c r="D115" s="11"/>
       <c r="E115" s="10"/>
     </row>
     <row r="116" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="10"/>
-      <c r="B116" s="26"/>
+      <c r="B116" s="29"/>
       <c r="C116" s="10"/>
       <c r="D116" s="11"/>
       <c r="E116" s="10"/>
@@ -2288,16 +2306,16 @@
       <c r="A117" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="27"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="28"/>
-      <c r="E117" s="29"/>
+      <c r="B117" s="24"/>
+      <c r="C117" s="25"/>
+      <c r="D117" s="25"/>
+      <c r="E117" s="26"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B118" s="24">
+      <c r="B118" s="27">
         <v>45441</v>
       </c>
       <c r="C118" s="5">
@@ -2312,7 +2330,7 @@
       <c r="A119" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B119" s="25"/>
+      <c r="B119" s="28"/>
       <c r="C119" s="8">
         <v>100</v>
       </c>
@@ -2325,7 +2343,7 @@
       <c r="A120" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B120" s="25"/>
+      <c r="B120" s="28"/>
       <c r="C120" s="8">
         <v>55</v>
       </c>
@@ -2338,7 +2356,7 @@
       <c r="A121" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B121" s="25"/>
+      <c r="B121" s="28"/>
       <c r="C121" s="8">
         <v>50</v>
       </c>
@@ -2351,7 +2369,7 @@
       <c r="A122" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B122" s="25"/>
+      <c r="B122" s="28"/>
       <c r="C122" s="10">
         <v>5</v>
       </c>
@@ -2362,50 +2380,136 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="21"/>
-      <c r="B123" s="25"/>
+      <c r="B123" s="28"/>
       <c r="C123" s="10"/>
       <c r="D123" s="11"/>
       <c r="E123" s="10"/>
     </row>
     <row r="124" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="10"/>
-      <c r="B124" s="26"/>
+      <c r="B124" s="29"/>
       <c r="C124" s="10"/>
       <c r="D124" s="11"/>
       <c r="E124" s="10"/>
     </row>
-    <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="32" t="s">
+    <row r="125" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B125" s="24"/>
+      <c r="C125" s="25"/>
+      <c r="D125" s="25"/>
+      <c r="E125" s="26"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B126" s="27">
+        <v>45442</v>
+      </c>
+      <c r="C126" s="5">
+        <v>70</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E126" s="10"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B127" s="28"/>
+      <c r="C127" s="8">
+        <v>20</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E127" s="22"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B128" s="28"/>
+      <c r="C128" s="8">
+        <v>50</v>
+      </c>
+      <c r="D128" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E128" s="8"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" s="28"/>
+      <c r="C129" s="8">
+        <v>35</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E129" s="22"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B130" s="28"/>
+      <c r="C130" s="10">
+        <v>5</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E130" s="10"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="21"/>
+      <c r="B131" s="28"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="11"/>
+      <c r="E131" s="10"/>
+    </row>
+    <row r="132" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="10"/>
+      <c r="B132" s="29"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="11"/>
+      <c r="E132" s="10"/>
+    </row>
+    <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="33"/>
-      <c r="C125" s="13">
-        <f>MROUND(SUM(C7:C36,C54:C124) /60,0.2)</f>
-        <v>69.2</v>
-      </c>
-      <c r="D125" s="14"/>
-      <c r="E125" s="15"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
+      <c r="B133" s="31"/>
+      <c r="C133" s="13">
+        <f>MROUND(SUM(C7:C36,C54:C132) /60,0.2)</f>
+        <v>72.2</v>
+      </c>
+      <c r="D133" s="14"/>
+      <c r="E133" s="15"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="16"/>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B109:E109"/>
-    <mergeCell ref="B110:B116"/>
-    <mergeCell ref="B101:E101"/>
-    <mergeCell ref="A125:B125"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:B12"/>
+  <mergeCells count="37">
+    <mergeCell ref="B126:B132"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B86:B92"/>
+    <mergeCell ref="B93:E93"/>
+    <mergeCell ref="B94:B100"/>
+    <mergeCell ref="B125:E125"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B45:E45"/>
     <mergeCell ref="B46:B52"/>
@@ -2413,27 +2517,33 @@
     <mergeCell ref="B21:B28"/>
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="B30:B36"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="B14:B19"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B109:E109"/>
+    <mergeCell ref="B110:B116"/>
+    <mergeCell ref="B101:E101"/>
+    <mergeCell ref="A133:B133"/>
     <mergeCell ref="B53:E53"/>
     <mergeCell ref="B54:B60"/>
     <mergeCell ref="B102:B108"/>
     <mergeCell ref="B117:E117"/>
     <mergeCell ref="B118:B124"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B14:B19"/>
     <mergeCell ref="B61:E61"/>
     <mergeCell ref="B62:B68"/>
     <mergeCell ref="B69:E69"/>
     <mergeCell ref="B70:B76"/>
     <mergeCell ref="B77:E77"/>
     <mergeCell ref="B78:B84"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B86:B92"/>
-    <mergeCell ref="B93:E93"/>
-    <mergeCell ref="B94:B100"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B118 C118:C124 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84 B86 C86:C92 B94 C94:C100 B102 C102:C108 B110 C110:C116">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B7 C7:C12 B14 B46 C14:C19 B21 C21:C28 B30 C30:C36 B38 C38:C44 B118 C46:C52 B54 C54:C60 B62 C62:C68 B70 C70:C76 B78 C78:C84 B86 C86:C92 B94 C94:C100 B102 C102:C108 B110 C110:C116 C118:C124 B126 C126:C132">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -2444,7 +2554,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="35" orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Etml_font,Normal"&amp;22ETML&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;14&amp;D&amp;R&amp;14Journal</oddFooter>
@@ -2463,17 +2573,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="c618a99f0a6dee3024750140ac9f5c62">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b661a4484808186e18f4202386b00979" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -2674,6 +2773,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="99ffe1f3-7857-457f-add0-5bdef636f38d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
   <ds:schemaRefs>
@@ -2683,23 +2793,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{852563C9-5FC3-4358-990E-BBE612A6AA36}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2716,4 +2809,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48045A0F-FB9C-4063-A5C2-24F6A995E167}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>